<commit_message>
updated results and data folders with new .csv files
</commit_message>
<xml_diff>
--- a/SimpleEnergyModel/Data_SimpleEnergyModel.xlsx
+++ b/SimpleEnergyModel/Data_SimpleEnergyModel.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184C7EC0-9939-5842-A7BD-81DADDEC911F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C0D24D-130D-5744-86F1-94A45C539B7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27700" windowHeight="16080" tabRatio="771" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27700" windowHeight="16080" tabRatio="771" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2 - Demands" sheetId="1" r:id="rId1"/>
-    <sheet name="3 - Primary Energy Supply" sheetId="2" r:id="rId2"/>
-    <sheet name="4 - EL supply (thermal and T&amp;D)" sheetId="3" r:id="rId3"/>
-    <sheet name="6 - EL supply (wind&amp;solar)" sheetId="5" r:id="rId4"/>
-    <sheet name="7 - Emissions" sheetId="7" r:id="rId5"/>
+    <sheet name="2 - Demands" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="2 - Demands_new" sheetId="8" r:id="rId2"/>
+    <sheet name="3 - Primary Energy Supply" sheetId="2" r:id="rId3"/>
+    <sheet name="4 - EL supply (thermal and T&amp;D)" sheetId="3" r:id="rId4"/>
+    <sheet name="6 - EL supply (wind&amp;solar)" sheetId="5" r:id="rId5"/>
+    <sheet name="7 - Emissions" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -22,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="64">
   <si>
     <t>SETS</t>
   </si>
@@ -654,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD56"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3778,6 +3782,1956 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6124D7D5-B23D-4F40-8057-561E876435E8}">
+  <dimension ref="A2:AD37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:AB22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>2014</v>
+      </c>
+      <c r="C6">
+        <v>2015</v>
+      </c>
+      <c r="D6">
+        <v>2016</v>
+      </c>
+      <c r="E6">
+        <v>2017</v>
+      </c>
+      <c r="F6">
+        <v>2018</v>
+      </c>
+      <c r="G6">
+        <v>2019</v>
+      </c>
+      <c r="H6">
+        <v>2020</v>
+      </c>
+      <c r="I6">
+        <v>2021</v>
+      </c>
+      <c r="J6">
+        <v>2022</v>
+      </c>
+      <c r="K6">
+        <v>2023</v>
+      </c>
+      <c r="L6">
+        <v>2024</v>
+      </c>
+      <c r="M6">
+        <v>2025</v>
+      </c>
+      <c r="N6">
+        <v>2026</v>
+      </c>
+      <c r="O6">
+        <v>2027</v>
+      </c>
+      <c r="P6">
+        <v>2028</v>
+      </c>
+      <c r="Q6">
+        <v>2029</v>
+      </c>
+      <c r="R6">
+        <v>2030</v>
+      </c>
+      <c r="S6">
+        <v>2031</v>
+      </c>
+      <c r="T6">
+        <v>2032</v>
+      </c>
+      <c r="U6">
+        <v>2033</v>
+      </c>
+      <c r="V6">
+        <v>2034</v>
+      </c>
+      <c r="W6">
+        <v>2035</v>
+      </c>
+      <c r="X6">
+        <v>2036</v>
+      </c>
+      <c r="Y6">
+        <v>2037</v>
+      </c>
+      <c r="Z6">
+        <v>2038</v>
+      </c>
+      <c r="AA6">
+        <v>2039</v>
+      </c>
+      <c r="AB6">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2022</v>
+      </c>
+      <c r="K11" s="1">
+        <v>2023</v>
+      </c>
+      <c r="L11" s="1">
+        <v>2024</v>
+      </c>
+      <c r="M11" s="1">
+        <v>2025</v>
+      </c>
+      <c r="N11" s="1">
+        <v>2026</v>
+      </c>
+      <c r="O11" s="1">
+        <v>2027</v>
+      </c>
+      <c r="P11" s="1">
+        <v>2028</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>2029</v>
+      </c>
+      <c r="R11" s="1">
+        <v>2030</v>
+      </c>
+      <c r="S11" s="1">
+        <v>2031</v>
+      </c>
+      <c r="T11" s="1">
+        <v>2032</v>
+      </c>
+      <c r="U11" s="1">
+        <v>2033</v>
+      </c>
+      <c r="V11" s="1">
+        <v>2034</v>
+      </c>
+      <c r="W11" s="1">
+        <v>2035</v>
+      </c>
+      <c r="X11" s="1">
+        <v>2036</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>2037</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>2038</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>2039</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="M12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="O12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="R12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="S12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="T12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="U12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="V12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="W12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="X12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="Y12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="Z12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="AA12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="AB12" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="C13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="D13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="E13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="F13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="G13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="H13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="I13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="K13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="L13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="M13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="N13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="O13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="P13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="R13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="S13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="T13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="U13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="V13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="W13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="X13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="Y13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="Z13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="AA13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="AB13" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="K14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="L14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="M14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="N14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="O14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="P14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="R14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="S14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="T14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="U14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="V14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="W14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="X14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="Y14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="Z14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="AA14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="AB14" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="C15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="D15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="E15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="F15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="G15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="H15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="I15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="K15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="L15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="M15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="N15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="O15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="P15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="R15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="S15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="T15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="U15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="V15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="W15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="X15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="Y15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="Z15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="AA15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="AB15" s="7">
+        <v>8.3299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="M16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="N16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="O16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="P16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="R16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="S16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="T16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="U16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="V16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="W16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="X16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="Y16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="Z16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="AA16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="AB16" s="7">
+        <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="M17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="N17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="O17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="P17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="R17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="S17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="T17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="U17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="V17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="W17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="X17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="Y17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="Z17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="AA17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="AB17" s="7">
+        <v>0.16669999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I21" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J21" s="1">
+        <v>2022</v>
+      </c>
+      <c r="K21" s="1">
+        <v>2023</v>
+      </c>
+      <c r="L21" s="1">
+        <v>2024</v>
+      </c>
+      <c r="M21" s="1">
+        <v>2025</v>
+      </c>
+      <c r="N21" s="1">
+        <v>2026</v>
+      </c>
+      <c r="O21" s="1">
+        <v>2027</v>
+      </c>
+      <c r="P21" s="1">
+        <v>2028</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>2029</v>
+      </c>
+      <c r="R21" s="1">
+        <v>2030</v>
+      </c>
+      <c r="S21" s="1">
+        <v>2031</v>
+      </c>
+      <c r="T21" s="1">
+        <v>2032</v>
+      </c>
+      <c r="U21" s="1">
+        <v>2033</v>
+      </c>
+      <c r="V21" s="1">
+        <v>2034</v>
+      </c>
+      <c r="W21" s="1">
+        <v>2035</v>
+      </c>
+      <c r="X21" s="1">
+        <v>2036</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>2037</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>2038</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>2039</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>2.214</v>
+      </c>
+      <c r="C22">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="D22">
+        <v>2.274</v>
+      </c>
+      <c r="E22">
+        <v>2.3420000000000001</v>
+      </c>
+      <c r="F22">
+        <v>2.726</v>
+      </c>
+      <c r="G22">
+        <v>2.9089999999999998</v>
+      </c>
+      <c r="H22">
+        <v>3.089</v>
+      </c>
+      <c r="I22">
+        <v>3.383</v>
+      </c>
+      <c r="J22">
+        <v>3.53</v>
+      </c>
+      <c r="K22">
+        <v>3.786</v>
+      </c>
+      <c r="L22">
+        <v>3.9050000000000002</v>
+      </c>
+      <c r="M22">
+        <v>4.0060000000000002</v>
+      </c>
+      <c r="N22">
+        <v>4.1609999999999996</v>
+      </c>
+      <c r="O22">
+        <v>4.3209999999999997</v>
+      </c>
+      <c r="P22">
+        <v>4.4359999999999999</v>
+      </c>
+      <c r="Q22">
+        <v>4.5380000000000003</v>
+      </c>
+      <c r="R22">
+        <v>4.6360000000000001</v>
+      </c>
+      <c r="S22">
+        <v>4.7690000000000001</v>
+      </c>
+      <c r="T22">
+        <v>5.0030000000000001</v>
+      </c>
+      <c r="U22">
+        <v>5.1390000000000002</v>
+      </c>
+      <c r="V22">
+        <v>5.2759999999999998</v>
+      </c>
+      <c r="W22">
+        <v>5.4029999999999996</v>
+      </c>
+      <c r="X22">
+        <v>5.5549999999999997</v>
+      </c>
+      <c r="Y22">
+        <v>5.7320000000000002</v>
+      </c>
+      <c r="Z22">
+        <v>5.9039999999999999</v>
+      </c>
+      <c r="AA22">
+        <v>6.0809999999999995</v>
+      </c>
+      <c r="AB22">
+        <v>6.3229999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2016</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2019</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I23" s="1">
+        <v>2021</v>
+      </c>
+      <c r="J23" s="1">
+        <v>2022</v>
+      </c>
+      <c r="K23" s="1">
+        <v>2023</v>
+      </c>
+      <c r="L23" s="1">
+        <v>2024</v>
+      </c>
+      <c r="M23" s="1">
+        <v>2025</v>
+      </c>
+      <c r="N23" s="1">
+        <v>2026</v>
+      </c>
+      <c r="O23" s="1">
+        <v>2027</v>
+      </c>
+      <c r="P23" s="1">
+        <v>2028</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>2029</v>
+      </c>
+      <c r="R23" s="1">
+        <v>2030</v>
+      </c>
+      <c r="S23" s="1">
+        <v>2031</v>
+      </c>
+      <c r="T23" s="1">
+        <v>2032</v>
+      </c>
+      <c r="U23" s="1">
+        <v>2033</v>
+      </c>
+      <c r="V23" s="1">
+        <v>2034</v>
+      </c>
+      <c r="W23" s="1">
+        <v>2035</v>
+      </c>
+      <c r="X23" s="1">
+        <v>2036</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>2037</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>2038</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>2039</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="I24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="J24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="K24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="L24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="M24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="N24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="O24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="P24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="R24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="S24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="T24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="U24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="V24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="W24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="X24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="Y24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="Z24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="AA24" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="AB24" s="7">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="G25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="I25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="J25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="K25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="L25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="M25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="N25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="O25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="P25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="R25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="S25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="T25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="U25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="V25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="W25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="X25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="Y25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="Z25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="AA25" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="AB25" s="7">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="H26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="J26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="K26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="L26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="M26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="N26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="O26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="P26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="R26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="S26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="T26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="U26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="V26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="W26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="X26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="Y26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="Z26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="AA26" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="AB26" s="7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="H27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="I27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="J27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="K27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="L27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="M27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="N27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="O27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="P27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="R27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="S27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="T27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="U27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="V27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="W27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="X27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="Y27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="Z27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="AA27" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="AB27" s="7">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="C28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="H28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="I28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="K28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="L28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="M28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="N28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="O28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="P28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="R28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="S28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="T28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="U28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="V28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="W28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="X28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="Y28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="Z28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA28" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AB28" s="7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="G29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="H29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="I29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="J29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="K29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="L29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="M29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="N29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="O29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="P29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="R29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="S29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="T29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="U29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="V29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="W29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="X29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="Y29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="Z29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AB29" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B33" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2015</v>
+      </c>
+      <c r="F33" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2017</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2018</v>
+      </c>
+      <c r="I33" s="1">
+        <v>2019</v>
+      </c>
+      <c r="J33" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K33" s="1">
+        <v>2021</v>
+      </c>
+      <c r="L33" s="1">
+        <v>2022</v>
+      </c>
+      <c r="M33" s="1">
+        <v>2023</v>
+      </c>
+      <c r="N33" s="1">
+        <v>2024</v>
+      </c>
+      <c r="O33" s="1">
+        <v>2025</v>
+      </c>
+      <c r="P33" s="1">
+        <v>2026</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>2027</v>
+      </c>
+      <c r="R33" s="1">
+        <v>2028</v>
+      </c>
+      <c r="S33" s="1">
+        <v>2029</v>
+      </c>
+      <c r="T33" s="1">
+        <v>2030</v>
+      </c>
+      <c r="U33" s="1">
+        <v>2031</v>
+      </c>
+      <c r="V33" s="1">
+        <v>2032</v>
+      </c>
+      <c r="W33" s="1">
+        <v>2033</v>
+      </c>
+      <c r="X33" s="1">
+        <v>2034</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>2035</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>2036</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>2037</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>2038</v>
+      </c>
+      <c r="AC33" s="1">
+        <v>2039</v>
+      </c>
+      <c r="AD33" s="1">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="E34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="F34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="G34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="H34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="I34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="J34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="K34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="L34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="M34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="N34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="O34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="P34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="Q34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="R34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="S34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="T34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="U34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="V34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="W34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="X34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="Y34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="Z34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="AA34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="AB34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="AC34" s="12">
+        <v>999999</v>
+      </c>
+      <c r="AD34" s="12">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="12">
+        <v>1</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="E35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="F35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="G35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="H35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="I35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="J35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="K35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="L35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="M35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="N35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="O35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="P35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="Q35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="R35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="S35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="T35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="U35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="V35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="W35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="X35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="Y35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="Z35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="AA35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="AB35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="AC35" s="12">
+        <v>999999</v>
+      </c>
+      <c r="AD35" s="12">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="12">
+        <v>1</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="12">
+        <v>1</v>
+      </c>
+      <c r="E36" s="12">
+        <v>1</v>
+      </c>
+      <c r="F36" s="12">
+        <v>1</v>
+      </c>
+      <c r="G36" s="12">
+        <v>1</v>
+      </c>
+      <c r="H36" s="12">
+        <v>1</v>
+      </c>
+      <c r="I36" s="12">
+        <v>1</v>
+      </c>
+      <c r="J36" s="12">
+        <v>1</v>
+      </c>
+      <c r="K36" s="12">
+        <v>1</v>
+      </c>
+      <c r="L36" s="12">
+        <v>1</v>
+      </c>
+      <c r="M36" s="12">
+        <v>1</v>
+      </c>
+      <c r="N36" s="12">
+        <v>1</v>
+      </c>
+      <c r="O36" s="12">
+        <v>1</v>
+      </c>
+      <c r="P36" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="12">
+        <v>1</v>
+      </c>
+      <c r="R36" s="12">
+        <v>1</v>
+      </c>
+      <c r="S36" s="12">
+        <v>1</v>
+      </c>
+      <c r="T36" s="12">
+        <v>1</v>
+      </c>
+      <c r="U36" s="12">
+        <v>1</v>
+      </c>
+      <c r="V36" s="12">
+        <v>1</v>
+      </c>
+      <c r="W36" s="12">
+        <v>1</v>
+      </c>
+      <c r="X36" s="12">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="12">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="12">
+        <v>1</v>
+      </c>
+      <c r="AA36" s="12">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="12">
+        <v>1</v>
+      </c>
+      <c r="AC36" s="12">
+        <v>1</v>
+      </c>
+      <c r="AD36" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:AE18"/>
   <sheetViews>
@@ -4549,7 +6503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:AE32"/>
   <sheetViews>
@@ -6227,11 +8181,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:AE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A37" sqref="A37:XFD41"/>
     </sheetView>
   </sheetViews>
@@ -8378,7 +10332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:AE13"/>
   <sheetViews>

</xml_diff>